<commit_message>
befor add time orders
</commit_message>
<xml_diff>
--- a/db/bin/real_trade_db_2024-09-12.xlsx
+++ b/db/bin/real_trade_db_2024-09-12.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z273"/>
+  <dimension ref="A1:Z274"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22461,7 +22461,7 @@
         </is>
       </c>
       <c r="D260" s="2" t="n">
-        <v>45547.1536629718</v>
+        <v>45547.15366297454</v>
       </c>
       <c r="E260" t="n">
         <v>198.14</v>
@@ -22543,7 +22543,7 @@
         </is>
       </c>
       <c r="D261" s="2" t="n">
-        <v>45547.15498265027</v>
+        <v>45547.15498265046</v>
       </c>
       <c r="E261" t="n">
         <v>160.2099</v>
@@ -22639,7 +22639,7 @@
         </is>
       </c>
       <c r="D262" s="2" t="n">
-        <v>45547.21324044037</v>
+        <v>45547.21324043981</v>
       </c>
       <c r="E262" t="n">
         <v>156.48</v>
@@ -22721,7 +22721,7 @@
         </is>
       </c>
       <c r="D263" s="2" t="n">
-        <v>45547.21333063965</v>
+        <v>45547.21333063657</v>
       </c>
       <c r="E263" t="n">
         <v>79.13</v>
@@ -22803,7 +22803,7 @@
         </is>
       </c>
       <c r="D264" s="2" t="n">
-        <v>45547.2134165144</v>
+        <v>45547.21341651621</v>
       </c>
       <c r="E264" t="n">
         <v>257.24</v>
@@ -22885,7 +22885,7 @@
         </is>
       </c>
       <c r="D265" s="2" t="n">
-        <v>45547.21349493817</v>
+        <v>45547.21349494213</v>
       </c>
       <c r="E265" t="n">
         <v>61.75</v>
@@ -22967,7 +22967,7 @@
         </is>
       </c>
       <c r="D266" s="2" t="n">
-        <v>45547.21368918075</v>
+        <v>45547.21368917824</v>
       </c>
       <c r="E266" t="n">
         <v>125.27</v>
@@ -23063,7 +23063,7 @@
         </is>
       </c>
       <c r="D267" s="2" t="n">
-        <v>45547.22109904797</v>
+        <v>45547.22109905093</v>
       </c>
       <c r="E267" t="n">
         <v>248.03</v>
@@ -23145,7 +23145,7 @@
         </is>
       </c>
       <c r="D268" s="2" t="n">
-        <v>45547.22652343502</v>
+        <v>45547.2265234375</v>
       </c>
       <c r="E268" t="n">
         <v>81.28</v>
@@ -23227,7 +23227,7 @@
         </is>
       </c>
       <c r="D269" s="2" t="n">
-        <v>45547.23111492278</v>
+        <v>45547.23111491898</v>
       </c>
       <c r="E269" t="n">
         <v>79.34999999999999</v>
@@ -23323,7 +23323,7 @@
         </is>
       </c>
       <c r="D270" s="2" t="n">
-        <v>45547.23275737058</v>
+        <v>45547.23275737269</v>
       </c>
       <c r="E270" t="n">
         <v>151.6893</v>
@@ -23419,7 +23419,7 @@
         </is>
       </c>
       <c r="D271" s="2" t="n">
-        <v>45547.23606039933</v>
+        <v>45547.23606040509</v>
       </c>
       <c r="E271" t="n">
         <v>263.3656</v>
@@ -23511,7 +23511,7 @@
         </is>
       </c>
       <c r="D272" s="2" t="n">
-        <v>45547.2438732927</v>
+        <v>45547.24387328704</v>
       </c>
       <c r="E272" t="n">
         <v>233.28</v>
@@ -23593,7 +23593,7 @@
         </is>
       </c>
       <c r="D273" s="2" t="n">
-        <v>45547.24432797147</v>
+        <v>45547.24432797453</v>
       </c>
       <c r="E273" t="n">
         <v>83.2</v>
@@ -23662,6 +23662,88 @@
         </is>
       </c>
     </row>
+    <row r="274">
+      <c r="A274" s="1" t="n">
+        <v>272</v>
+      </c>
+      <c r="B274" t="n">
+        <v>0</v>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>SPG</t>
+        </is>
+      </c>
+      <c r="D274" s="2" t="n">
+        <v>45547.9868338868</v>
+      </c>
+      <c r="E274" t="n">
+        <v>161.51</v>
+      </c>
+      <c r="F274" t="n">
+        <v>2099.63</v>
+      </c>
+      <c r="G274" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H274" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I274" t="inlineStr"/>
+      <c r="J274" t="n">
+        <v>0</v>
+      </c>
+      <c r="K274" t="n">
+        <v>0</v>
+      </c>
+      <c r="L274" t="n">
+        <v>13</v>
+      </c>
+      <c r="M274" t="inlineStr">
+        <is>
+          <t>cancelled</t>
+        </is>
+      </c>
+      <c r="N274" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O274" t="n">
+        <v>0.995</v>
+      </c>
+      <c r="P274" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q274" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R274" t="n">
+        <v>0</v>
+      </c>
+      <c r="S274" t="inlineStr">
+        <is>
+          <t>FA19747A91177B2000</t>
+        </is>
+      </c>
+      <c r="T274" t="inlineStr"/>
+      <c r="U274" t="inlineStr"/>
+      <c r="V274" t="inlineStr"/>
+      <c r="W274" t="inlineStr"/>
+      <c r="X274" t="inlineStr">
+        <is>
+          <t>1m</t>
+        </is>
+      </c>
+      <c r="Y274" t="inlineStr">
+        <is>
+          <t>mv :-1.05, mv_2m:0.92,  mv_5m : -1.39, mv_30m : -0.39, mv_60m: -0.39</t>
+        </is>
+      </c>
+      <c r="Z274" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>